<commit_message>
73. Set Matrix Zeroes
73. Set Matrix Zeroes
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Array\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840C94F1-1B59-499F-83CB-748316962824}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B62E343-28B3-40D0-8FD4-FF126DC0FC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Leetcode</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Palindrome String</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes</t>
   </si>
 </sst>
 </file>
@@ -369,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,6 +407,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1920. Build Array from Permutation
1920. Build Array from Permutation
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Array\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B62E343-28B3-40D0-8FD4-FF126DC0FC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE137B2-A661-4743-BC50-B99CFE2C0943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Leetcode</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>Build Array from Permutation</t>
   </si>
 </sst>
 </file>
@@ -86,12 +89,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,12 +393,12 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>344</v>
       </c>
       <c r="B2" t="s">
@@ -400,7 +406,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -408,11 +414,19 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1920</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Leetcode and GFG problem from DSA-450
Leetcode and GFG problem from DSA-450
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE137B2-A661-4743-BC50-B99CFE2C0943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA83FFF-F76F-45C1-B1C4-575864C0C40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Leetcode</t>
   </si>
@@ -46,6 +46,27 @@
   </si>
   <si>
     <t>Build Array from Permutation</t>
+  </si>
+  <si>
+    <t>Minimize the Heights II</t>
+  </si>
+  <si>
+    <t>Minimize the Heights I</t>
+  </si>
+  <si>
+    <t>Find minimum and maximum element in an array</t>
+  </si>
+  <si>
+    <t>Kth smallest element</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Java</t>
   </si>
 </sst>
 </file>
@@ -89,14 +110,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -378,55 +404,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="53.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>344</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>73</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>1920</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>215</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
39.Combination sum in subset and 78.subset
39.Combination sum in subset and 78.subset
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA83FFF-F76F-45C1-B1C4-575864C0C40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3437E7-83F5-420D-B97C-EEE1395DEF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Leetcode</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Java</t>
+  </si>
+  <si>
+    <t>Combination Sum</t>
+  </si>
+  <si>
+    <t>Subsets</t>
   </si>
 </sst>
 </file>
@@ -110,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -124,6 +130,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,19 +414,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>344</v>
       </c>
@@ -435,7 +446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -443,7 +454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>73</v>
       </c>
@@ -451,7 +462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1920</v>
       </c>
@@ -459,7 +470,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -470,7 +481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -481,7 +492,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -492,7 +503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -503,7 +514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>215</v>
       </c>
@@ -512,6 +523,34 @@
       </c>
       <c r="C10" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="6">
+        <v>44982</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="6">
+        <v>44981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GFG. Print sum of all subset
GFG. Print sum of all subset
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3437E7-83F5-420D-B97C-EEE1395DEF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167036B9-35D4-4C42-8FFA-E96FF82722CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Leetcode</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Subsets</t>
+  </si>
+  <si>
+    <t>Print sum of all subset</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +556,20 @@
         <v>44981</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="6">
+        <v>44983</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG. Array subset of another array
GFG. Array subset of another array
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A635481A-502B-473C-8FE6-C3C50CD322B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9980EDD4-0C51-4EF7-8620-F7BD5C5AAE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Leetcode</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Subsets II</t>
+  </si>
+  <si>
+    <t>Array Subset of another array</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,6 +590,20 @@
         <v>44984</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="6">
+        <v>44985</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
189. Rotate Array to right by K
189. Rotate Array to right by K
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7223A0C0-1015-4554-B1D2-9364089DA7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1C22A5-D104-4F02-9A61-87CE2D03D6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Leetcode</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Sort Colors</t>
+  </si>
+  <si>
+    <t>Rotate Array to right by K</t>
   </si>
 </sst>
 </file>
@@ -427,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,6 +625,20 @@
         <v>44986</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>189</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="6">
+        <v>44992</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG. Largest Element in Array
GFG. Largest Element in Array
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1C22A5-D104-4F02-9A61-87CE2D03D6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB7442D-0ECF-4D2C-A80A-1E0792F665D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Leetcode</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Rotate Array to right by K</t>
+  </si>
+  <si>
+    <t>Largest Element in Array</t>
   </si>
 </sst>
 </file>
@@ -430,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,8 +629,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>189</v>
+      <c r="A17" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
@@ -637,6 +640,20 @@
       </c>
       <c r="D17" s="6">
         <v>44992</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="6">
+        <v>45000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GFG. Second Largest in Array
GFG. Second Largest in Array
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB7442D-0ECF-4D2C-A80A-1E0792F665D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31B29C7-EC24-4010-9CE4-40BB961F55FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>Leetcode</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Largest Element in Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Second Largest in Array</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,6 +659,20 @@
         <v>45000</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="6">
+        <v>45000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG. Cyclically rotate an array by one
GFG. Cyclically rotate an array by one
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31B29C7-EC24-4010-9CE4-40BB961F55FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C973EE-C818-4173-A9D3-FB9FEA16B033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>Leetcode</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Second Largest in Array</t>
+  </si>
+  <si>
+    <t>Cyclically rotate an array by one</t>
   </si>
 </sst>
 </file>
@@ -436,17 +439,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -673,6 +676,20 @@
         <v>45000</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="6">
+        <v>45000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
26. Remove Duplicates from Sorted Array 1752.Check if array is Sorted and Rotated
26. Remove Duplicates from Sorted Array
1752.Check if array is Sorted and Rotated
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C973EE-C818-4173-A9D3-FB9FEA16B033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5969A9DE-3CF4-4275-A0EA-97C848F5495C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Leetcode</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Cyclically rotate an array by one</t>
+  </si>
+  <si>
+    <t>Check if Array Is Sorted and Rotated</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,6 +696,34 @@
         <v>45000</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>1752</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="6">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="6">
+        <v>45000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG. Rotate Array to left by K
GFG. Rotate Array to left by K
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5969A9DE-3CF4-4275-A0EA-97C848F5495C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DE3FE4-6814-4ACA-95B5-19A8ACADDAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>Leetcode</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Remove Duplicates from Sorted Array</t>
+  </si>
+  <si>
+    <t>Rotate Array  to left by K</t>
   </si>
 </sst>
 </file>
@@ -126,12 +129,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -146,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -165,6 +174,10 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,10 +654,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="A17" s="8">
+        <v>189</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
@@ -721,6 +734,20 @@
         <v>13</v>
       </c>
       <c r="D22" s="6">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="6">
         <v>45000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GFG. Move all zeros to end of array and searching an element in a sorted array
GFG. Move all zeros to end of array and searching an element in a sorted array
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DE3FE4-6814-4ACA-95B5-19A8ACADDAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4127B2D0-9DF6-4ED2-A25E-0B6B193A293C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Leetcode</t>
   </si>
@@ -106,13 +106,19 @@
   </si>
   <si>
     <t>Rotate Array  to left by K</t>
+  </si>
+  <si>
+    <t>Move all zeroes to end of array</t>
+  </si>
+  <si>
+    <t>Searching an element in a sorted array</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +129,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -155,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -178,6 +192,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="C25" sqref="C25:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +768,34 @@
         <v>45000</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="6">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="6">
+        <v>45000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
349. Intersection of Two Array and GFG. Union of Two sorted array
349. Intersection of Two Array and GFG. Union of Two sorted array
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4127B2D0-9DF6-4ED2-A25E-0B6B193A293C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D79DA7E-8CC8-485C-BF5C-AA2F084ED60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>Leetcode</t>
   </si>
@@ -112,13 +112,19 @@
   </si>
   <si>
     <t>Searching an element in a sorted array</t>
+  </si>
+  <si>
+    <t>Union of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t>Intersection of Two Arrays</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,14 +135,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -169,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -192,9 +190,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:D25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,17 +777,45 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" t="s">
         <v>28</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="6">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="6">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>349</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="6">
         <v>45000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
485. Max Consecutive Ones
485. Max Consecutive Ones
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4545BF1-E35D-4A22-8D99-EE649DAF1576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5531BC9F-DF20-4F75-95B2-E68F754DE935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>Leetcode</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t xml:space="preserve">Java </t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones</t>
   </si>
 </sst>
 </file>
@@ -476,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,6 +842,20 @@
         <v>45000</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>485</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="6">
+        <v>45003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Coding Ninja-Longest subarray with Sum k-Part 1 and 2.
Coding Ninja-Longest subarray with Sum k-Part 1 and 2.
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2748562D-1A20-4ABF-A110-D35BD86CD918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCF1804-2E0E-47EA-90E8-E8D900E164B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>Leetcode</t>
   </si>
@@ -130,6 +141,58 @@
   </si>
   <si>
     <t>Single Number</t>
+  </si>
+  <si>
+    <t>Ninja</t>
+  </si>
+  <si>
+    <t>Longest Subarray With Sum K</t>
+  </si>
+  <si>
+    <t>Longest Subarray With Sum K.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0&lt;=A[i]&lt;=10^9 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>It will work for +ve elements in an array</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>For +ve and -ve values of element in array and K</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -153,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -202,6 +271,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:D30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,20 +575,27 @@
     <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>344</v>
       </c>
@@ -514,7 +603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -522,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>73</v>
       </c>
@@ -530,7 +619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1920</v>
       </c>
@@ -538,7 +627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -549,7 +638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -560,7 +649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -571,7 +660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -582,7 +671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>215</v>
       </c>
@@ -593,7 +682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>39</v>
       </c>
@@ -607,7 +696,7 @@
         <v>44982</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>78</v>
       </c>
@@ -621,7 +710,7 @@
         <v>44981</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
@@ -635,7 +724,7 @@
         <v>44983</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>90</v>
       </c>
@@ -649,7 +738,7 @@
         <v>44984</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
@@ -663,7 +752,7 @@
         <v>44985</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>75</v>
       </c>
@@ -677,21 +766,21 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>189</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="C17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="14">
         <v>44992</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
@@ -705,7 +794,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
@@ -719,7 +808,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>3</v>
       </c>
@@ -733,7 +822,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>1752</v>
       </c>
@@ -747,7 +836,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>26</v>
       </c>
@@ -761,21 +850,21 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="6">
+      <c r="C23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="14">
         <v>45000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>3</v>
       </c>
@@ -789,7 +878,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>3</v>
       </c>
@@ -803,7 +892,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
@@ -817,7 +906,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>349</v>
       </c>
@@ -831,7 +920,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>268</v>
       </c>
@@ -845,7 +934,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>485</v>
       </c>
@@ -859,7 +948,7 @@
         <v>45003</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>136</v>
       </c>
@@ -871,6 +960,40 @@
       </c>
       <c r="D30" s="6">
         <v>45003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="12">
+        <v>45003</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="12">
+        <v>45003</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ninja. Longest Subarray with sum k- optimal solution
Ninja. Longest Subarray with sum k- optimal solution
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCF1804-2E0E-47EA-90E8-E8D900E164B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1BD9CB-1531-45DF-AC68-6E0C918CD878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -248,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -284,6 +284,9 @@
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,7 +570,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +966,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="11" t="s">
@@ -980,7 +983,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="11" t="s">

</xml_diff>

<commit_message>
GFG.Longest Sub-Array with Sum K
GFG.Longest Sub-Array with Sum K
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1BD9CB-1531-45DF-AC68-6E0C918CD878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7EE9E3-7852-43F3-8FDF-361A29B01C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>Leetcode</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Longest Sub-Array with Sum K</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,6 +1002,23 @@
         <v>39</v>
       </c>
     </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="12">
+        <v>45003</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG. Find all pairs with a given sum
GFG. Find all pairs with a given sum
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CEE43E-775C-4492-AD7F-2D0E0033E3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD09E47-ED6A-4823-9D02-651BDC4E184F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
   <si>
     <t>Leetcode</t>
   </si>
@@ -200,6 +200,9 @@
   <si>
     <t>Two Sum</t>
   </si>
+  <si>
+    <t>Find all pairs with a given sum</t>
+  </si>
 </sst>
 </file>
 
@@ -222,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +244,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -254,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -292,6 +301,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,16 +1040,30 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+      <c r="A34" s="18">
         <v>1</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="6">
+      <c r="C34" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="20">
+        <v>45006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="20">
         <v>45006</v>
       </c>
     </row>

</xml_diff>

<commit_message>
121. Best Time to Buy and Sell Stock
121. Best Time to Buy and Sell Stock
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D6782F-1B7E-47F9-B438-91952E06B7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6D7B8C-2084-4DE7-A255-86B775DEA0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
   <si>
     <t>Leetcode</t>
   </si>
@@ -212,6 +212,12 @@
   <si>
     <t>53/GFG</t>
   </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>The GFG Q has problem try only LC</t>
+  </si>
 </sst>
 </file>
 
@@ -234,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +265,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -274,16 +286,10 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -306,8 +312,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -322,6 +326,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,74 +614,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="53.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="22" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>344</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>73</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>1920</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
@@ -677,10 +689,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
@@ -688,10 +700,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
@@ -699,10 +711,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
@@ -710,10 +722,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>215</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
@@ -721,7 +733,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>39</v>
       </c>
       <c r="B11" t="s">
@@ -730,12 +742,12 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>44982</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>78</v>
       </c>
       <c r="B12" t="s">
@@ -744,26 +756,26 @@
       <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>44981</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <v>44983</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="3">
         <v>90</v>
       </c>
       <c r="B14" t="s">
@@ -772,26 +784,26 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <v>44984</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="4">
         <v>44985</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="3">
         <v>75</v>
       </c>
       <c r="B16" t="s">
@@ -800,26 +812,26 @@
       <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="5">
         <v>44986</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="6">
         <v>189</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="14">
+      <c r="C17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="12">
         <v>44992</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
@@ -828,12 +840,12 @@
       <c r="C18" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="4">
         <v>45000</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B19" t="s">
@@ -842,12 +854,12 @@
       <c r="C19" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="4">
         <v>45000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
@@ -856,12 +868,12 @@
       <c r="C20" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="4">
         <v>45000</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="3">
         <v>1752</v>
       </c>
       <c r="B21" t="s">
@@ -870,12 +882,12 @@
       <c r="C21" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="4">
         <v>45000</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="3">
         <v>26</v>
       </c>
       <c r="B22" t="s">
@@ -884,26 +896,26 @@
       <c r="C22" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="4">
         <v>45000</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="14">
+      <c r="C23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="12">
         <v>45000</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B24" t="s">
@@ -912,12 +924,12 @@
       <c r="C24" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="4">
         <v>45000</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B25" t="s">
@@ -926,12 +938,12 @@
       <c r="C25" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="4">
         <v>45000</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B26" t="s">
@@ -940,12 +952,12 @@
       <c r="C26" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>45000</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="3">
         <v>349</v>
       </c>
       <c r="B27" t="s">
@@ -954,12 +966,12 @@
       <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="4">
         <v>45000</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="3">
         <v>268</v>
       </c>
       <c r="B28" t="s">
@@ -968,12 +980,12 @@
       <c r="C28" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <v>45000</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="3">
         <v>485</v>
       </c>
       <c r="B29" t="s">
@@ -982,12 +994,12 @@
       <c r="C29" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <v>45003</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="3">
         <v>136</v>
       </c>
       <c r="B30" t="s">
@@ -996,115 +1008,132 @@
       <c r="C30" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="4">
         <v>45003</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="10">
         <v>45003</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="10">
         <v>45003</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="11" t="s">
+      <c r="A33" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="10">
         <v>45003</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="18">
+      <c r="A34" s="14">
         <v>1</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="20">
+      <c r="C34" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="16">
         <v>45006</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="21" t="s">
+      <c r="A35" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="20">
+      <c r="C35" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="16">
         <v>45006</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
+      <c r="A36" s="3">
         <v>169</v>
       </c>
       <c r="B36" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="7">
+      <c r="C36" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="5">
         <v>45019</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B37" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="7">
+      <c r="C37" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="5">
         <v>45020</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>121</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="5">
+        <v>45020</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2149. Rearrange Array Elements by Sign and GFG. Alternate positive and negative numbers
2149. Rearrange Array Elements by Sign
GFG. Alternate positive and negative numbers
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6D7B8C-2084-4DE7-A255-86B775DEA0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA5DCE0-EE7A-495D-92C7-1935182104E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
   <si>
     <t>Leetcode</t>
   </si>
@@ -218,6 +218,18 @@
   <si>
     <t>The GFG Q has problem try only LC</t>
   </si>
+  <si>
+    <t>Rearrange Array Elements by Sign</t>
+  </si>
+  <si>
+    <t>Alternate positive and negative numbers</t>
+  </si>
+  <si>
+    <t>Varitey 1- where +ve and -ve are same in number</t>
+  </si>
+  <si>
+    <t>Varitey 2- where +ve and -ve are not in number</t>
+  </si>
 </sst>
 </file>
 
@@ -240,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +283,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -284,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -334,6 +352,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +649,7 @@
     <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="54.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1136,6 +1160,40 @@
         <v>49</v>
       </c>
     </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="23">
+        <v>2149</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="25">
+        <v>45021</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="25">
+        <v>45021</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG. Leaders in an array
GFG. Leaders in an array
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA5DCE0-EE7A-495D-92C7-1935182104E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE7512F-C911-460F-A96D-304C460FB38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
   <si>
     <t>Leetcode</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Varitey 2- where +ve and -ve are not in number</t>
+  </si>
+  <si>
+    <t>Leaders in an array</t>
   </si>
 </sst>
 </file>
@@ -302,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -358,6 +361,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,6 +1200,20 @@
         <v>53</v>
       </c>
     </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="4">
+        <v>45022</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
128. Longest Consecutive Sequence
128. Longest Consecutive Sequence
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7DF36F-7DFC-4753-821C-15B44FA042C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0046DF84-2BC4-4F77-BE60-43A50AEFE76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>Leetcode</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>Next Permutation</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <t>128/GFG</t>
   </si>
 </sst>
 </file>
@@ -647,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,6 +1237,20 @@
         <v>45023</v>
       </c>
     </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="4">
+        <v>45023</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
229. Majority Element II
229. Majority Element II
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3803385-DAB6-4FFF-94C3-FE0434B39100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D8B836-4CF7-4F58-8201-DCF794541FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="60">
   <si>
     <t>Leetcode</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Rotate Image</t>
+  </si>
+  <si>
+    <t>Majority Element II</t>
   </si>
 </sst>
 </file>
@@ -656,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,6 +1285,20 @@
         <v>45026</v>
       </c>
     </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>229</v>
+      </c>
+      <c r="B46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="4">
+        <v>45031</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
560. Subarray Sum equals K and Subarray  with XOR 'K'
560. Subarray Sum equals K and Subarray  with XOR 'K'
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66E7268-C026-4928-AD5B-C47B63578752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83D3C48-D84E-4F78-8AB8-9436149D48D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
   <si>
     <t>Leetcode</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>Spiral Matrix</t>
+  </si>
+  <si>
+    <t>Subarray Sum Equals K</t>
+  </si>
+  <si>
+    <t>Subarrays with XOR ‘K’</t>
+  </si>
+  <si>
+    <t>Coding Ninja</t>
   </si>
 </sst>
 </file>
@@ -677,15 +686,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="54.28515625" style="8" customWidth="1"/>
@@ -1365,6 +1374,34 @@
         <v>45037</v>
       </c>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>560</v>
+      </c>
+      <c r="B50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="4">
+        <v>45049</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="4">
+        <v>45049</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Leetcode-56,88 and GFG-Missing and repeating number and merge an array without an extra space
Leetcode-56,88 and GFG-Missing and repeating number and merge an array without an extra space
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83D3C48-D84E-4F78-8AB8-9436149D48D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456A86A6-0CC6-43C0-978A-ACAB29865E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
   <si>
     <t>Leetcode</t>
   </si>
@@ -272,6 +272,21 @@
   <si>
     <t>Coding Ninja</t>
   </si>
+  <si>
+    <t>Merge Intervals</t>
+  </si>
+  <si>
+    <t>Merge Without Extra Space</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>Here we need to merge everything and put it in the first array</t>
+  </si>
+  <si>
+    <t>Find Missing And Repeating</t>
+  </si>
 </sst>
 </file>
 
@@ -294,7 +309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +346,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -344,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -406,6 +427,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,7 +1386,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>54</v>
       </c>
@@ -1374,7 +1400,7 @@
         <v>45037</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>560</v>
       </c>
@@ -1388,7 +1414,7 @@
         <v>45049</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>67</v>
       </c>
@@ -1400,6 +1426,65 @@
       </c>
       <c r="D51" s="4">
         <v>45049</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>56</v>
+      </c>
+      <c r="B52" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="4">
+        <v>45054</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="29">
+        <v>88</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="31">
+        <v>45054</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="31">
+        <v>45054</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="4">
+        <v>45054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
152. Maximum Product Subarray
152. Maximum Product Subarray
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456A86A6-0CC6-43C0-978A-ACAB29865E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6480E2-8C41-4DE1-BA6C-E66F83B8C8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="74">
   <si>
     <t>Leetcode</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>Find Missing And Repeating</t>
+  </si>
+  <si>
+    <t>Maximum Product Subarray</t>
   </si>
 </sst>
 </file>
@@ -712,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,6 +1490,20 @@
         <v>45054</v>
       </c>
     </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>152</v>
+      </c>
+      <c r="B56" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="5">
+        <v>45057</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated 27 Aug 2023
updated 27 Aug 2023
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Array\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6480E2-8C41-4DE1-BA6C-E66F83B8C8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A066E402-50A7-48FB-8CE6-52DC44C314EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
   <si>
     <t>Leetcode</t>
   </si>
@@ -290,6 +279,82 @@
   <si>
     <t>Maximum Product Subarray</t>
   </si>
+  <si>
+    <t>GFG/Coding Ninja</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Brute force</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-sort the arr and the last element is the largest element,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Better solution-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> does not exits,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Optimal solution-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> we need to compare each element in the array and return the largest element at last but we need to cover an edge case where the arr has only one element.</t>
+    </r>
+  </si>
+  <si>
+    <t>IN Coding ninja problem use set function to insert the element and not add it will give wrong ans</t>
+  </si>
 </sst>
 </file>
 
@@ -312,7 +377,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +420,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -368,73 +439,113 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="15" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,792 +826,802 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="54.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="53.88671875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="11.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="54.33203125" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>344</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>73</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1920</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>215</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15">
         <v>44982</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>78</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="15">
         <v>44981</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="15">
         <v>44983</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>90</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15">
         <v>44984</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="15">
         <v>44985</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>75</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="16">
         <v>44986</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>189</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="12">
+      <c r="C17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="17">
         <v>44992</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="13">
         <v>45000</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="E18" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="4">
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="15">
         <v>45000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="15">
         <v>45000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>1752</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="4">
+      <c r="C21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="15">
         <v>45000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="4">
+      <c r="C22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="11">
         <v>45000</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="7" t="s">
+      <c r="E22" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="12">
+      <c r="C23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="17">
         <v>45000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="15">
         <v>45000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="4">
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="15">
         <v>45000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="4">
+      <c r="C26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="15">
         <v>45000</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
         <v>349</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="4">
+      <c r="C27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="15">
         <v>45000</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
         <v>268</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="15">
         <v>45000</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
         <v>485</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="15">
         <v>45003</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
         <v>136</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="15">
         <v>45003</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="18">
         <v>45003</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="18">
         <v>45003</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="33" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="9" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="18">
         <v>45003</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="33" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
         <v>1</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="16">
+      <c r="C34" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="19">
         <v>45006</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="17" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="16">
+      <c r="C35" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="19">
         <v>45006</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
         <v>169</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="5">
+      <c r="C36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="16">
         <v>45019</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="5">
+      <c r="C37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="16">
         <v>45020</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>121</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="5">
+      <c r="C38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="16">
         <v>45020</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="31" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="23">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
         <v>2149</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="25">
+      <c r="C39" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="20">
         <v>45021</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="E39" s="34" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="24" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="25">
+      <c r="C40" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="20">
         <v>45021</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="34" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="27" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="4">
+      <c r="C41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="15">
         <v>45022</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
         <v>31</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="4">
+      <c r="C42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="15">
         <v>45023</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="4">
+      <c r="C43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="15">
         <v>45023</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
         <v>73</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C44" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="4">
+      <c r="C44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="15">
         <v>45026</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
         <v>48</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="4">
+      <c r="C45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="15">
         <v>45026</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
         <v>229</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="15">
         <v>45031</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="14">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="5">
         <v>15</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="16">
+      <c r="D47" s="19">
         <v>45031</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="35" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="28">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="8">
         <v>18</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="16">
+      <c r="C48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="19">
         <v>45036</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E48" s="35" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
         <v>54</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="4">
+      <c r="C49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="15">
         <v>45037</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
         <v>560</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="4">
+      <c r="C50" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="15">
         <v>45049</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="4">
+      <c r="C51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="15">
         <v>45049</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
         <v>56</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C52" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="4">
+      <c r="C52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="15">
         <v>45054</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="29">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="9">
         <v>88</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" s="31">
+      <c r="C53" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="21">
         <v>45054</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B54" s="30" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="31">
+      <c r="C54" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="21">
         <v>45054</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C55" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" s="4">
+      <c r="C55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="15">
         <v>45054</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
         <v>152</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C56" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="5">
+      <c r="C56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="16">
         <v>45057</v>
       </c>
     </row>

</xml_diff>

<commit_message>
75. Sort Colors (Sort 0s,1s,2s)
Documentation updated
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6957C015-8AE6-4DC5-8C7B-8CE7B10E7942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3601F0B9-F4C4-4578-A389-14D5F0381CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="85">
   <si>
     <t>Leetcode</t>
   </si>
@@ -485,6 +485,78 @@
       </rPr>
       <t>1.We need to sort the array
 2. we will use 2 pointer approach where we will place left pointer at start and right pointer at the end and will add both the element and check if it matches with target if it is less than target we will move the left pointer and if it is more than target we will move the right pointer.</t>
+    </r>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Brute Force-
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Using a sorting Algo like Merge Sort but TC--&gt;O(NlogN)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Better Approach-
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Using 3 counter and counting how many number of 0,1 and 2 are present and then running a loop and changing the main array based on the three counters.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Optimal Approach</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-Dutch National Flag</t>
     </r>
   </si>
 </sst>
@@ -509,7 +581,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -561,6 +633,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -742,68 +820,75 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1087,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1101,7 +1186,7 @@
     <col min="6" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1203,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>344</v>
       </c>
@@ -1126,7 +1211,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1134,7 +1219,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>73</v>
       </c>
@@ -1142,7 +1227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1920</v>
       </c>
@@ -1150,7 +1235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1161,7 +1246,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -1172,7 +1257,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1183,7 +1268,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
@@ -1194,7 +1279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>215</v>
       </c>
@@ -1205,7 +1290,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>39</v>
       </c>
@@ -1219,7 +1304,7 @@
         <v>44982</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>78</v>
       </c>
@@ -1233,7 +1318,7 @@
         <v>44981</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>3</v>
       </c>
@@ -1247,7 +1332,7 @@
         <v>44983</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>90</v>
       </c>
@@ -1261,7 +1346,7 @@
         <v>44984</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>3</v>
       </c>
@@ -1275,18 +1360,24 @@
         <v>44985</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
+    <row r="16" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
         <v>75</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="14">
+      <c r="C16" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="63">
         <v>44986</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="61" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1546,7 +1637,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="41" customFormat="1" ht="239.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="40" customFormat="1" ht="239.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="36">
         <v>1</v>
       </c>
@@ -1562,15 +1653,15 @@
       <c r="E34" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="60" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="41" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="40" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="41" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="38" t="s">
@@ -1580,7 +1671,7 @@
         <v>45006</v>
       </c>
       <c r="E35" s="39"/>
-      <c r="F35" s="40"/>
+      <c r="F35" s="60"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
@@ -1628,36 +1719,36 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="43">
+      <c r="A39" s="42">
         <v>2149</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="46">
+      <c r="C39" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="45">
         <v>45021</v>
       </c>
-      <c r="E39" s="47" t="s">
+      <c r="E39" s="46" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="46">
+      <c r="C40" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="45">
         <v>45021</v>
       </c>
-      <c r="E40" s="47" t="s">
+      <c r="E40" s="46" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1746,19 +1837,19 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="48">
+      <c r="A47" s="47">
         <v>15</v>
       </c>
       <c r="B47" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="49" t="s">
+      <c r="C47" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="49">
+      <c r="D47" s="48">
         <v>45031</v>
       </c>
-      <c r="E47" s="50" t="s">
+      <c r="E47" s="49" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1769,13 +1860,13 @@
       <c r="B48" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="49">
+      <c r="C48" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="48">
         <v>45036</v>
       </c>
-      <c r="E48" s="50" t="s">
+      <c r="E48" s="49" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1836,16 +1927,16 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="52">
+      <c r="A53" s="51">
         <v>88</v>
       </c>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" s="55">
+      <c r="C53" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="54">
         <v>45054</v>
       </c>
       <c r="E53" s="9" t="s">
@@ -1853,16 +1944,16 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="52" t="s">
+      <c r="A54" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="53" t="s">
+      <c r="B54" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="55">
+      <c r="C54" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="54">
         <v>45054</v>
       </c>
     </row>
@@ -1894,23 +1985,23 @@
         <v>45057</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="60" customFormat="1" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="56">
+    <row r="57" spans="1:6" s="59" customFormat="1" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="55">
         <v>283</v>
       </c>
-      <c r="B57" s="57" t="s">
+      <c r="B57" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="C57" s="58" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="58" t="s">
+      <c r="C57" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="E57" s="59" t="s">
+      <c r="E57" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="F57" s="60" t="s">
+      <c r="F57" s="59" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GFG. Leaders in array
Documentation update
</commit_message>
<xml_diff>
--- a/Array/Question_Array.xlsx
+++ b/Array/Question_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3601F0B9-F4C4-4578-A389-14D5F0381CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493A875A-1370-425F-9024-DA7ADECDD7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
   <si>
     <t>Leetcode</t>
   </si>
@@ -557,6 +557,83 @@
         <scheme val="minor"/>
       </rPr>
       <t>-Dutch National Flag</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Brute Force-
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Using two for loop, pick element and compare with the entire array and increment the count once the inner loop end compare the counter if it is &gt;N/2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.Better Approach-
+3. Optimal Approach- 
+Using Moore Voting Algorithm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1. Brute Force-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Using two for loop we will check each element with the one in right and add it to leader list or AL.TC--&gt; O(N)2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. Optimal Approach- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+We will iterate from back and check the element with maxi where maxi is given minimum value if the element is greater than maxi then its the highest among the element to its right.Depending on answer we will return the list if needed sorted or the order needs to be maintained.</t>
     </r>
   </si>
 </sst>
@@ -707,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -880,14 +957,17 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1172,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,13 +1450,13 @@
       <c r="C16" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="63">
+      <c r="D16" s="62">
         <v>44986</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="61" t="s">
+      <c r="F16" s="60" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1653,7 +1733,7 @@
       <c r="E34" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="60" t="s">
+      <c r="F34" s="64" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1671,10 +1751,10 @@
         <v>45006</v>
       </c>
       <c r="E35" s="39"/>
-      <c r="F35" s="60"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="13">
+      <c r="F35" s="64"/>
+    </row>
+    <row r="36" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="6">
         <v>169</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -1683,8 +1763,11 @@
       <c r="C36" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="14">
+      <c r="D36" s="62">
         <v>45019</v>
+      </c>
+      <c r="E36" s="63" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1752,9 +1835,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
-        <v>3</v>
+    <row r="41" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>54</v>
@@ -1764,6 +1847,9 @@
       </c>
       <c r="D41" s="12">
         <v>45022</v>
+      </c>
+      <c r="E41" s="61" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>